<commit_message>
Aula 2 - calculos estátiscicos, gráficos e desafio
Atualização dos gráficos na aba análises
</commit_message>
<xml_diff>
--- a/Imersão Python - Tabela de ações.xlsx
+++ b/Imersão Python - Tabela de ações.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\OneDrive - UNINTER - Aluno\Minha Biblioteca\Imersão Python (Alura)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{5BAAEFE0-F9F2-4888-B662-CFDE43B28998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54EE82AB-DF6C-4278-A55D-C88ACB65E30E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA47C9-B50E-4CBD-BF7E-F919776B09DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="1" r:id="rId1"/>
@@ -19,35 +19,24 @@
     <sheet name="ChatGPT" sheetId="5" r:id="rId4"/>
     <sheet name="Análises" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -4904,6 +4893,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4919,6 +4913,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4934,6 +4933,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4949,6 +4953,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -4964,6 +4973,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -4979,6 +4993,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -4996,6 +5015,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -5013,6 +5037,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -5030,6 +5059,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -5047,6 +5081,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -5064,6 +5103,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -5081,6 +5125,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -5099,6 +5148,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -5117,6 +5171,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -5135,6 +5194,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -5153,6 +5217,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -5171,6 +5240,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -5189,6 +5263,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="18"/>
@@ -5206,6 +5285,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="19"/>
@@ -5223,6 +5307,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -5240,6 +5329,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="21"/>
@@ -5257,6 +5351,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="22"/>
@@ -5274,6 +5373,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002D-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="23"/>
@@ -5291,6 +5395,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002F-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="24"/>
@@ -5309,6 +5418,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000031-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="25"/>
@@ -5327,6 +5441,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000033-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="26"/>
@@ -5345,6 +5464,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="27"/>
@@ -5363,6 +5487,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000037-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="28"/>
@@ -5381,6 +5510,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000039-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="29"/>
@@ -5399,6 +5533,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003B-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="30"/>
@@ -5416,6 +5555,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003D-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="31"/>
@@ -5433,6 +5577,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003F-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="32"/>
@@ -5450,6 +5599,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000041-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="33"/>
@@ -5467,6 +5621,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000043-B4CD-440B-A230-3566975299BA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -5741,7 +5900,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5771,7 +5930,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5847,7 +6006,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5909,7 +6068,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-BR"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -6033,7 +6192,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="651005959"/>
@@ -6092,7 +6251,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="175385095"/>
@@ -6134,7 +6293,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6171,7 +6330,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6203,13 +6362,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -6222,7 +6387,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="1"/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6235,19 +6400,25 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6273,13 +6444,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -6324,6 +6524,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -6331,7 +6532,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
         <c:axId val="311236616"/>
         <c:axId val="311250952"/>
       </c:barChart>
@@ -6346,9 +6548,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -6357,7 +6559,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="&quot;R$&quot;\ #,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -6374,9 +6576,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -6384,7 +6585,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="311236616"/>
@@ -6399,16 +6600,16 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -6422,9 +6623,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -6432,7 +6632,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="311250952"/>
@@ -6450,22 +6650,63 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -6476,7 +6717,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6494,10 +6735,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -6508,7 +6749,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6540,7 +6781,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6552,7 +6793,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6561,7 +6802,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="percentStacked"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -6579,7 +6820,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -6587,6 +6828,60 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Análises!$A$68:$A$70</c:f>
@@ -6629,34 +6924,35 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="79"/>
         <c:overlap val="100"/>
         <c:axId val="133289479"/>
         <c:axId val="311294984"/>
       </c:barChart>
-      <c:catAx>
-        <c:axId val="133289479"/>
+      <c:valAx>
+        <c:axId val="311294984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
+              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -6682,45 +6978,34 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311294984"/>
+        <c:crossAx val="133289479"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="311294984"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="133289479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -6729,7 +7014,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6741,13 +7026,16 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133289479"/>
+        <c:crossAx val="311294984"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6756,44 +7044,13 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -6813,7 +7070,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6905,12 +7162,9 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -6945,42 +7199,8 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="22">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -8012,7 +8232,503 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="298">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8023,7 +8739,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -8046,18 +8762,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -8069,19 +8785,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -8113,35 +8826,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8153,30 +8876,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8198,15 +8925,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -8216,7 +8941,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -8225,14 +8950,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8241,17 +8965,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -8260,10 +8983,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -8279,21 +9002,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -8312,17 +9029,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -8331,17 +9047,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -8350,17 +9065,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -8381,7 +9095,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -8389,148 +9103,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -8552,372 +9128,16 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -8938,7 +9158,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -8947,14 +9167,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -8968,27 +9188,26 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9002,6 +9221,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9009,14 +9239,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9061,16 +9285,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9101,15 +9325,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9139,16 +9363,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9481,39 +9705,39 @@
   </sheetPr>
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="12" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="22" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.42578125" style="11" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" style="20" customWidth="1"/>
     <col min="11" max="11" width="20.28515625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" style="22" customWidth="1"/>
     <col min="13" max="13" width="19.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17" style="20" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="22" customWidth="1"/>
     <col min="18" max="18" width="20.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" style="37" customWidth="1"/>
     <col min="20" max="20" width="18.140625" style="20" customWidth="1"/>
     <col min="21" max="21" width="18" style="20" customWidth="1"/>
-    <col min="22" max="22" width="20" style="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21" style="22" customWidth="1"/>
     <col min="23" max="23" width="20.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.140625" style="37" customWidth="1"/>
     <col min="25" max="25" width="18.140625" style="20" customWidth="1"/>
     <col min="26" max="26" width="18" style="20" customWidth="1"/>
-    <col min="27" max="27" width="20" style="22" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="21.42578125" style="22" customWidth="1"/>
     <col min="28" max="28" width="20.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.140625" style="54" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11.5703125" style="54" bestFit="1" customWidth="1"/>
@@ -18289,19 +18513,19 @@
         <v>-1.07</v>
       </c>
       <c r="E66" s="20">
-        <f t="shared" ref="E66:E97" si="29">D66/100</f>
+        <f t="shared" ref="E66:E82" si="29">D66/100</f>
         <v>-1.0700000000000001E-2</v>
       </c>
       <c r="F66" s="21">
-        <f t="shared" ref="F66:F97" si="30">C66/(E66+1)</f>
+        <f t="shared" ref="F66:F82" si="30">C66/(E66+1)</f>
         <v>16.668351359547152</v>
       </c>
       <c r="G66" s="22">
-        <f t="shared" ref="G66:G97" si="31">(C66-F66)*AF66</f>
+        <f t="shared" ref="G66:G82" si="31">(C66-F66)*AF66</f>
         <v>-42951047.215599783</v>
       </c>
       <c r="H66" s="25" t="str">
-        <f t="shared" ref="H66:H97" si="32">IF(G66&gt;0,"Subiu",IF(G66&lt;0,"Desceu","Estável"))</f>
+        <f t="shared" ref="H66:H82" si="32">IF(G66&gt;0,"Subiu",IF(G66&lt;0,"Desceu","Estável"))</f>
         <v>Desceu</v>
       </c>
       <c r="I66" s="15">
@@ -18320,7 +18544,7 @@
         <v>40875021.136080652</v>
       </c>
       <c r="M66" s="25" t="str">
-        <f t="shared" ref="M66:M97" si="33">IF(L66&gt;0,"Subiu",IF(L66&lt;0,"Desceu","Estável"))</f>
+        <f t="shared" ref="M66:M82" si="33">IF(L66&gt;0,"Subiu",IF(L66&lt;0,"Desceu","Estável"))</f>
         <v>Subiu</v>
       </c>
       <c r="N66" s="29">
@@ -18339,7 +18563,7 @@
         <v>-373179212.0529933</v>
       </c>
       <c r="R66" s="25" t="str">
-        <f t="shared" ref="R66:R97" si="34">IF(Q66&gt;0,"Subiu",IF(Q66&lt;0,"Desceu","Estável"))</f>
+        <f t="shared" ref="R66:R82" si="34">IF(Q66&gt;0,"Subiu",IF(Q66&lt;0,"Desceu","Estável"))</f>
         <v>Desceu</v>
       </c>
       <c r="S66" s="36">
@@ -18358,7 +18582,7 @@
         <v>-373179212.0529933</v>
       </c>
       <c r="W66" s="25" t="str">
-        <f t="shared" ref="W66:W97" si="35">IF(V66&gt;0,"Subiu",IF(V66&lt;0,"Desceu","Estável"))</f>
+        <f t="shared" ref="W66:W82" si="35">IF(V66&gt;0,"Subiu",IF(V66&lt;0,"Desceu","Estável"))</f>
         <v>Desceu</v>
       </c>
       <c r="X66" s="36">
@@ -18377,7 +18601,7 @@
         <v>581642200.72745275</v>
       </c>
       <c r="AB66" s="25" t="str">
-        <f t="shared" ref="AB66:AB97" si="36">IF(AA66&gt;0,"Subiu",IF(AA66&lt;0,"Desceu","Estável"))</f>
+        <f t="shared" ref="AB66:AB82" si="36">IF(AA66&gt;0,"Subiu",IF(AA66&lt;0,"Desceu","Estável"))</f>
         <v>Subiu</v>
       </c>
       <c r="AC66" s="36">
@@ -34169,7 +34393,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -64332,7 +64556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C38C4E-8833-4497-8B1F-91A8332FE5C1}">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
@@ -65495,8 +65719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371BD8BC-593A-486E-AB40-804405F47325}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C67" activeCellId="1" sqref="A67:A70 C67:C70"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="V79" sqref="V79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>